<commit_message>
added expected required circle count computation
</commit_message>
<xml_diff>
--- a/Examples/RKWithPoly/rk with poly and bnb/cnt.xlsx
+++ b/Examples/RKWithPoly/rk with poly and bnb/cnt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PyCharm_Projects\fire\Examples\RKWithPoly\rk with poly and bnb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80C0772-8970-4176-A4E7-18A8D87346BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C291D94-7F21-482E-9C79-8061A6203EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>P1</t>
   </si>
@@ -90,14 +90,43 @@
   </si>
   <si>
     <t>AVG Total:</t>
+  </si>
+  <si>
+    <t>achieved</t>
+  </si>
+  <si>
+    <t>theoretical</t>
+  </si>
+  <si>
+    <t>вот тут ему точно мало</t>
+  </si>
+  <si>
+    <t>кружкам прямо тяжело</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>weighted 4:1</t>
+  </si>
+  <si>
+    <t>нижнее подчёркивание - смог покрыть с таким числом кругов</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -211,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -233,6 +262,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -513,15 +551,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="G9" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -541,7 +579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -565,7 +603,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -589,7 +627,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -613,7 +651,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -637,7 +675,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -661,7 +699,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -685,7 +723,7 @@
         <v>13.100000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -716,7 +754,7 @@
         <v>10.485714285714284</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -730,12 +768,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -754,8 +792,26 @@
       <c r="J15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>19</v>
+      </c>
+      <c r="W15" t="s">
+        <v>18</v>
+      </c>
+      <c r="X15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -778,8 +834,38 @@
         <f>H16+I16</f>
         <v>6.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O16" t="str">
+        <f>A16</f>
+        <v>P1</v>
+      </c>
+      <c r="P16" s="1">
+        <f>C16</f>
+        <v>7</v>
+      </c>
+      <c r="Q16" s="22">
+        <v>5</v>
+      </c>
+      <c r="R16" t="s">
+        <v>24</v>
+      </c>
+      <c r="V16" t="str">
+        <f>A16</f>
+        <v>P1</v>
+      </c>
+      <c r="W16" s="1">
+        <v>5</v>
+      </c>
+      <c r="X16" s="27">
+        <v>5</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>8</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -802,8 +888,36 @@
         <f t="shared" ref="J17:J22" si="1">H17+I17</f>
         <v>3.3000000000000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O17" t="str">
+        <f t="shared" ref="O17:O22" si="2">A17</f>
+        <v>P2</v>
+      </c>
+      <c r="P17" s="4">
+        <f>C17</f>
+        <v>4</v>
+      </c>
+      <c r="Q17" s="23">
+        <v>4</v>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" ref="V17:V22" si="3">A17</f>
+        <v>P2</v>
+      </c>
+      <c r="W17" s="4">
+        <f t="shared" ref="W17:W22" si="4">C17</f>
+        <v>4</v>
+      </c>
+      <c r="X17" s="28">
+        <v>4</v>
+      </c>
+      <c r="Y17" s="25">
+        <v>9</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -826,8 +940,39 @@
         <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O18" t="str">
+        <f t="shared" si="2"/>
+        <v>P3</v>
+      </c>
+      <c r="P18" s="9">
+        <f>C18</f>
+        <v>9</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>7</v>
+      </c>
+      <c r="R18" t="s">
+        <v>20</v>
+      </c>
+      <c r="V18" t="str">
+        <f t="shared" si="3"/>
+        <v>P3</v>
+      </c>
+      <c r="W18" s="4">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="X18" s="26">
+        <v>7</v>
+      </c>
+      <c r="Y18" s="25">
+        <v>11</v>
+      </c>
+      <c r="Z18" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -850,8 +995,36 @@
         <f t="shared" si="1"/>
         <v>6.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O19" t="str">
+        <f t="shared" si="2"/>
+        <v>P4</v>
+      </c>
+      <c r="P19" s="4">
+        <f>C19</f>
+        <v>16</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>13</v>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" si="3"/>
+        <v>P4</v>
+      </c>
+      <c r="W19" s="4">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="X19" s="26">
+        <v>13</v>
+      </c>
+      <c r="Y19" s="25">
+        <v>22</v>
+      </c>
+      <c r="Z19" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -874,8 +1047,35 @@
         <f t="shared" si="1"/>
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O20" t="str">
+        <f t="shared" si="2"/>
+        <v>P7</v>
+      </c>
+      <c r="P20" s="4">
+        <f>C20</f>
+        <v>7</v>
+      </c>
+      <c r="Q20" s="23">
+        <v>6</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="3"/>
+        <v>P7</v>
+      </c>
+      <c r="W20" s="4">
+        <v>6</v>
+      </c>
+      <c r="X20" s="28">
+        <v>6</v>
+      </c>
+      <c r="Y20" s="25">
+        <v>11</v>
+      </c>
+      <c r="Z20" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -898,8 +1098,39 @@
         <f t="shared" si="1"/>
         <v>7.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O21" t="str">
+        <f t="shared" si="2"/>
+        <v>P8</v>
+      </c>
+      <c r="P21" s="4">
+        <f>C21</f>
+        <v>14</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>11</v>
+      </c>
+      <c r="S21" t="s">
+        <v>21</v>
+      </c>
+      <c r="V21" t="str">
+        <f t="shared" si="3"/>
+        <v>P8</v>
+      </c>
+      <c r="W21" s="4">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="X21" s="26">
+        <v>11</v>
+      </c>
+      <c r="Y21" s="25">
+        <v>20</v>
+      </c>
+      <c r="Z21" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -929,8 +1160,35 @@
         <f>AVERAGE(J16:J22)</f>
         <v>4.5285714285714294</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O22" t="str">
+        <f t="shared" si="2"/>
+        <v>P9</v>
+      </c>
+      <c r="P22" s="6">
+        <f>C22</f>
+        <v>3</v>
+      </c>
+      <c r="Q22" s="24">
+        <v>3</v>
+      </c>
+      <c r="V22" t="str">
+        <f t="shared" si="3"/>
+        <v>P9</v>
+      </c>
+      <c r="W22" s="6">
+        <v>3</v>
+      </c>
+      <c r="X22" s="29">
+        <v>3</v>
+      </c>
+      <c r="Y22" s="7">
+        <v>5</v>
+      </c>
+      <c r="Z22" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -944,7 +1202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>16</v>
       </c>

</xml_diff>